<commit_message>
upgraded to new framework
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SubsetModuleTest.xlsx
+++ b/resources/ExcelsheetData/SubsetModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="createSubsets" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="TC_Subset_10" sheetId="5" r:id="rId6"/>
     <sheet name="TC_Subset_11" sheetId="6" r:id="rId7"/>
     <sheet name="TC_Subset_12" sheetId="7" r:id="rId8"/>
+    <sheet name="TC_Subset_24" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>Sl. No</t>
   </si>
@@ -71,9 +72,6 @@
     <t>Update Message</t>
   </si>
   <si>
-    <t>Auto_EditSubset1</t>
-  </si>
-  <si>
     <t>Updated Successfully</t>
   </si>
   <si>
@@ -83,12 +81,6 @@
     <t>Brand Name</t>
   </si>
   <si>
-    <t>Automation_Manu001_Brand001</t>
-  </si>
-  <si>
-    <t>Automation_Manufacturer_001</t>
-  </si>
-  <si>
     <t>saveMessage</t>
   </si>
   <si>
@@ -111,6 +103,30 @@
   </si>
   <si>
     <t>userName</t>
+  </si>
+  <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>TC_Subset_09</t>
+  </si>
+  <si>
+    <t>AutomationTestSubsetEdit</t>
+  </si>
+  <si>
+    <t>unilog123#</t>
+  </si>
+  <si>
+    <t>AutomationTestManufacturer</t>
+  </si>
+  <si>
+    <t>AutomationTestBrand</t>
+  </si>
+  <si>
+    <t>TC_Subset_24</t>
   </si>
 </sst>
 </file>
@@ -133,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +159,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,12 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -651,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
@@ -693,10 +716,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -704,10 +727,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -736,10 +759,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -750,13 +773,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -766,22 +789,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,16 +813,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -806,13 +839,22 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -822,32 +864,46 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -857,46 +913,60 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -906,53 +976,109 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>